<commit_message>
testando o novo plot
</commit_message>
<xml_diff>
--- a/dados/estados_siglas.xlsx
+++ b/dados/estados_siglas.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\covidmetrika\COVID-19\Dashboard\aplicativo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\covidMetrika\dashboard_brasil\dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="63">
   <si>
     <t>Estado</t>
   </si>
@@ -190,6 +190,24 @@
   </si>
   <si>
     <t>Codigo</t>
+  </si>
+  <si>
+    <t>Norte</t>
+  </si>
+  <si>
+    <t>Nordeste</t>
+  </si>
+  <si>
+    <t>Sudeste</t>
+  </si>
+  <si>
+    <t>Sul</t>
+  </si>
+  <si>
+    <t>Centro-Oeste</t>
+  </si>
+  <si>
+    <t>Regiao</t>
   </si>
 </sst>
 </file>
@@ -497,15 +515,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" customHeight="1">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -515,8 +533,11 @@
       <c r="C1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="14.25">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -526,8 +547,11 @@
       <c r="C2">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="14.25">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -537,8 +561,11 @@
       <c r="C3">
         <v>27</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="14.25">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -548,8 +575,11 @@
       <c r="C4">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="14.25">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
@@ -559,8 +589,11 @@
       <c r="C5">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="14.25">
       <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
@@ -570,8 +603,11 @@
       <c r="C6">
         <v>29</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="D6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="14.25">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
@@ -581,8 +617,11 @@
       <c r="C7">
         <v>23</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="14.25">
       <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
@@ -592,8 +631,11 @@
       <c r="C8">
         <v>53</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="D8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="14.25">
       <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
@@ -603,8 +645,11 @@
       <c r="C9">
         <v>32</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="D9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="14.25">
       <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
@@ -614,8 +659,11 @@
       <c r="C10">
         <v>52</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="D10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="14.25">
       <c r="A11" s="3" t="s">
         <v>20</v>
       </c>
@@ -625,8 +673,11 @@
       <c r="C11">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="D11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="14.25">
       <c r="A12" s="3" t="s">
         <v>22</v>
       </c>
@@ -636,8 +687,11 @@
       <c r="C12">
         <v>51</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
+      <c r="D12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="14.25">
       <c r="A13" s="3" t="s">
         <v>24</v>
       </c>
@@ -647,8 +701,11 @@
       <c r="C13">
         <v>50</v>
       </c>
-    </row>
-    <row r="14" spans="1:3">
+      <c r="D13" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="14.25">
       <c r="A14" s="3" t="s">
         <v>26</v>
       </c>
@@ -658,8 +715,11 @@
       <c r="C14">
         <v>31</v>
       </c>
-    </row>
-    <row r="15" spans="1:3">
+      <c r="D14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="14.25">
       <c r="A15" s="3" t="s">
         <v>28</v>
       </c>
@@ -669,8 +729,11 @@
       <c r="C15">
         <v>15</v>
       </c>
-    </row>
-    <row r="16" spans="1:3">
+      <c r="D15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="14.25">
       <c r="A16" s="3" t="s">
         <v>30</v>
       </c>
@@ -680,8 +743,11 @@
       <c r="C16">
         <v>25</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="D16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="14.25">
       <c r="A17" s="3" t="s">
         <v>32</v>
       </c>
@@ -691,8 +757,11 @@
       <c r="C17">
         <v>41</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="D17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="14.25">
       <c r="A18" s="3" t="s">
         <v>34</v>
       </c>
@@ -702,8 +771,11 @@
       <c r="C18">
         <v>26</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="D18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="14.25">
       <c r="A19" s="3" t="s">
         <v>36</v>
       </c>
@@ -713,8 +785,11 @@
       <c r="C19">
         <v>22</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="D19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="14.25">
       <c r="A20" s="3" t="s">
         <v>38</v>
       </c>
@@ -724,8 +799,11 @@
       <c r="C20">
         <v>33</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
+      <c r="D20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="14.25">
       <c r="A21" s="3" t="s">
         <v>40</v>
       </c>
@@ -735,8 +813,11 @@
       <c r="C21">
         <v>24</v>
       </c>
-    </row>
-    <row r="22" spans="1:3">
+      <c r="D21" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="14.25">
       <c r="A22" s="3" t="s">
         <v>42</v>
       </c>
@@ -746,8 +827,11 @@
       <c r="C22">
         <v>43</v>
       </c>
-    </row>
-    <row r="23" spans="1:3">
+      <c r="D22" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="14.25">
       <c r="A23" s="3" t="s">
         <v>44</v>
       </c>
@@ -757,8 +841,11 @@
       <c r="C23">
         <v>11</v>
       </c>
-    </row>
-    <row r="24" spans="1:3">
+      <c r="D23" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="14.25">
       <c r="A24" s="3" t="s">
         <v>46</v>
       </c>
@@ -768,8 +855,11 @@
       <c r="C24">
         <v>14</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" ht="14.25">
+      <c r="D24" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="14.25">
       <c r="A25" s="3" t="s">
         <v>48</v>
       </c>
@@ -779,8 +869,11 @@
       <c r="C25">
         <v>42</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" ht="14.25">
+      <c r="D25" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="14.25">
       <c r="A26" s="3" t="s">
         <v>50</v>
       </c>
@@ -790,8 +883,11 @@
       <c r="C26">
         <v>35</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" ht="14.25">
+      <c r="D26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="14.25">
       <c r="A27" s="3" t="s">
         <v>52</v>
       </c>
@@ -801,8 +897,11 @@
       <c r="C27">
         <v>28</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" ht="14.25">
+      <c r="D27" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="14.25">
       <c r="A28" s="3" t="s">
         <v>54</v>
       </c>
@@ -812,8 +911,14 @@
       <c r="C28">
         <v>17</v>
       </c>
+      <c r="D28" t="s">
+        <v>57</v>
+      </c>
     </row>
   </sheetData>
+  <sortState ref="A2:D28">
+    <sortCondition ref="A1"/>
+  </sortState>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="A3" r:id="rId2"/>

</xml_diff>